<commit_message>
Added Transition - Chapter 2 Act 3
</commit_message>
<xml_diff>
--- a/GD1/GD1.xlsx
+++ b/GD1/GD1.xlsx
@@ -1491,8 +1491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added some effects, Some Notes to Excel
</commit_message>
<xml_diff>
--- a/GD1/GD1.xlsx
+++ b/GD1/GD1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="101">
   <si>
     <t>Name</t>
   </si>
@@ -275,14 +275,82 @@
     <t xml:space="preserve">Knowing there is resistance to the ISIS amongst the former professionals, doctors, and businessmen in the city you proceed to the former literature markets where thinkers and professionals continue to socialize. While drinking tea at a cafe you meet a former professor from the local university who offers you a room in his house. You tell him you ran a hookah cafe in town until the morality police shut it down and your family has since escaped the country. </t>
   </si>
   <si>
-    <t>--&gt; Chapter 2</t>
+    <t>--&gt; Chapter 3</t>
+  </si>
+  <si>
+    <t>Chapter One</t>
+  </si>
+  <si>
+    <t>These need to be organized</t>
+  </si>
+  <si>
+    <t>1. My deceased father moved here when he married my mother and so I picked up his accent...
+2. I don't understand. This is the way I speak. I cannot help it.
+3. I came here to ask for a loan, not to be questioned like some criminal. I am leaving!</t>
+  </si>
+  <si>
+    <t>1. Success ---&gt; (2) [The loan denied but he is allowed to leave]
+2. FAIL ---&gt; (3)[The armed man blocks the exit]
+3. FAIL ---&gt; (3)[The armed man blocks the exit]</t>
+  </si>
+  <si>
+    <t>STORY: Accent</t>
+  </si>
+  <si>
+    <t>SUCCESS</t>
+  </si>
+  <si>
+    <t>GREEN goes to a bank currently under ISIS control under the pretence of needing to borrow money. This gains him access to the backrooms where he can see large palletts of money are stored. The money collected from the people suffering under ISIS rule in order to be "redistributed to the poor". GREEN is led to a room where he meets with the bank manager a tallman in islamic attire... possibly  an ex-fighter. The man begins to ask GREEN for the reasons he needs a loan and about what he does for work and where he grew up. The officer gives GREEN a very disapproving look and  says "If you are a local, then why do you not speak with a local accent?" GREEN begins to panic, he did not expect his arabic skills, learnt from living in a neighbouring country, to out him as a spy. He scrambles to come up with an answer... "Well ... you see ..."</t>
+  </si>
+  <si>
+    <t>The acting bank manager ponders GREEN's response for a long minute. Then gets up and leaves, returning ten minutes later.... Very well then, our interview has be completed, but a loan will not be possible at this time. There is an enemy we must fight everyday, you would be much better suited to fighting with us against our enemies instead of opening a business.</t>
+  </si>
+  <si>
+    <t>CONTINUE</t>
+  </si>
+  <si>
+    <t>Go to next act/story</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The bank manager, whose face grows more twisted as GREEN attempts to pass it off as an insignificant observation, stands up quickly. Clearly offended by GREEN's response he calls for the guards. "You dare defy me and treat me for a fool? You are clearly not who you say you are. I cannot allow you to leave."
+GREEN is mortified as he tries to think of a way to diffuse this situation but within seconds, two young men carrying rifles, enter the room and begin to drag him out by his elbows. GREEN begs to be let go but it is no use. He is imprisoned and tortured. Though they are unable to break him, eventually  they decide to leave him to rot in a jail cell in one of the many underground jail cells until they figure out who he really is. MISSION FAILED. </t>
+  </si>
+  <si>
+    <t>Game Over</t>
+  </si>
+  <si>
+    <t>STORY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GREEN needs to contact his handlers back at the regional headquarters to update them on the situation and request a new local to be paired with. So GREEN goes out and purchases a cheap phone from the local bazaar with some prepaid minutes. In case his phone call is triangulated he finds some privacy in an alley behind one of the busy streets and makes a quick call to HQ and leaves a coded message. His handlers will know that his local partner has been compromised. Within 30 seconds of making the call he hangs up to make it difficult for his call to be traced. He returns home while waiting for a call back. Several hours later his phone rings. </t>
+  </si>
+  <si>
+    <t>Go to 2 (continue story)</t>
+  </si>
+  <si>
+    <t>Go to 3 (continue story)</t>
+  </si>
+  <si>
+    <t>GREEN is told his new handler is a widow whose husband, a prominent politician, was shot at his office by ISIS soon after they took over the city. She used to run a clothing stall but since the occupation, women are not allowed to work. Green is told to show up at a local park just before the sun begins to set and look for a women reading a book. Then he is told to ask her for directions, listen for the response "It is just a short walk away, follow true north" and then walk away. She will then get up and leave and he is to follow her.</t>
+  </si>
+  <si>
+    <t>GREEN arrives at the park just before the sun begins to go down, knowing that most people would be in a hurry to make it to the nearest mosque for prayers they would be paid little attention and the park wouldn't be too busy. There he sees BLUE and he walks up to her and asks for directions to the local mosque. After a moment of silence, BLUE gives him the cryptic response and he thanks her and walks away. Moments later he follows her to a house on a quiet street, by now most people ought to be praying and wouldn't notice him. He enters the house.</t>
+  </si>
+  <si>
+    <t>Go to 4</t>
+  </si>
+  <si>
+    <t>Once inside the home, BLUE takes off her niqab and greets him in broken english. They exchange names and she prepares some tea. In a hushed voice she tells him about how ISIS organizes all the different city departments now and what she thinks are strategic targets to gather intelligence on. They spend hours plotting, before he lives under the shadow of darkness. The frequent electricity shortages means whole neighbourhoods are often shrouded in pitch darkness.</t>
+  </si>
+  <si>
+    <t>next story</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -305,8 +373,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -343,6 +433,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="19">
     <border>
@@ -550,7 +652,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -605,6 +707,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -628,6 +742,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1030,8 +1153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C20"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,7 +1316,7 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="J6" sqref="J6:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1210,22 +1333,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="E1" s="36" t="s">
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="E1" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="38"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="42"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
@@ -1296,11 +1419,11 @@
       <c r="M5" s="20"/>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
       <c r="E6" s="22" t="s">
         <v>48</v>
       </c>
@@ -1310,7 +1433,7 @@
       <c r="I6" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="J6" s="41" t="s">
+      <c r="J6" s="45" t="s">
         <v>61</v>
       </c>
       <c r="K6" s="19"/>
@@ -1318,9 +1441,9 @@
       <c r="M6" s="20"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
+      <c r="A7" s="44"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
       <c r="E7" s="24"/>
       <c r="F7" s="25" t="s">
         <v>56</v>
@@ -1332,7 +1455,7 @@
         <v>57</v>
       </c>
       <c r="I7" s="19"/>
-      <c r="J7" s="41"/>
+      <c r="J7" s="45"/>
       <c r="K7" s="21" t="s">
         <v>64</v>
       </c>
@@ -1344,9 +1467,9 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
+      <c r="A8" s="44"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
       <c r="E8" s="24"/>
       <c r="F8" s="23"/>
       <c r="G8" s="23"/>
@@ -1354,7 +1477,7 @@
       <c r="I8" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="J8" s="41"/>
+      <c r="J8" s="45"/>
       <c r="K8" s="19"/>
       <c r="L8" s="19"/>
       <c r="M8" s="29" t="s">
@@ -1362,9 +1485,9 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
+      <c r="A9" s="44"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
       <c r="E9" s="24"/>
       <c r="F9" s="23"/>
       <c r="G9" s="23"/>
@@ -1374,16 +1497,16 @@
       <c r="K9" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="L9" s="34" t="s">
+      <c r="L9" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="M9" s="35"/>
+      <c r="M9" s="39"/>
       <c r="N9" s="17"/>
     </row>
     <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="40"/>
-      <c r="B10" s="40"/>
-      <c r="C10" s="40"/>
+      <c r="A10" s="44"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
       <c r="E10" s="30"/>
       <c r="F10" s="31"/>
       <c r="G10" s="31"/>
@@ -1395,84 +1518,84 @@
       <c r="M10" s="32"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="40"/>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
+      <c r="A11" s="44"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
+      <c r="A12" s="44"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
+      <c r="A13" s="44"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="40"/>
+      <c r="A14" s="44"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="40"/>
+      <c r="A15" s="44"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
+      <c r="A16" s="44"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
+      <c r="A17" s="44"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="40"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
+      <c r="A19" s="44"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="40"/>
-      <c r="B20" s="40"/>
-      <c r="C20" s="40"/>
+      <c r="A20" s="44"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="40"/>
-      <c r="B21" s="40"/>
-      <c r="C21" s="40"/>
+      <c r="A21" s="44"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="44"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="40"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="40"/>
+      <c r="A22" s="44"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="44"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="40"/>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
+      <c r="A23" s="44"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="40"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
+      <c r="A24" s="44"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="40"/>
-      <c r="B25" s="40"/>
-      <c r="C25" s="40"/>
+      <c r="A25" s="44"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="44"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="40"/>
-      <c r="B26" s="40"/>
-      <c r="C26" s="40"/>
+      <c r="A26" s="44"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1489,15 +1612,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E11"/>
+  <dimension ref="A3:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="58.5703125" style="9" customWidth="1"/>
     <col min="4" max="4" width="45.140625" style="9" customWidth="1"/>
@@ -1505,24 +1628,24 @@
     <col min="6" max="16384" width="17.5703125" style="9"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="34" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -1538,8 +1661,11 @@
       <c r="E4" s="9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="F4" s="46" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -1555,8 +1681,9 @@
       <c r="E5" s="9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="F5" s="46"/>
+    </row>
+    <row r="6" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -1572,8 +1699,9 @@
       <c r="E6" s="9" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="F6" s="46"/>
+    </row>
+    <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -1589,8 +1717,9 @@
       <c r="E7" s="9" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="F7" s="46"/>
+    </row>
+    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -1606,8 +1735,9 @@
       <c r="E8" s="9" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="F8" s="46"/>
+    </row>
+    <row r="9" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>6</v>
       </c>
@@ -1623,8 +1753,9 @@
       <c r="E9" s="9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="F9" s="46"/>
+    </row>
+    <row r="10" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>7</v>
       </c>
@@ -1640,8 +1771,9 @@
       <c r="E10" s="9" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="F10" s="46"/>
+    </row>
+    <row r="11" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>8</v>
       </c>
@@ -1657,8 +1789,183 @@
       <c r="E11" s="33" t="s">
         <v>79</v>
       </c>
+      <c r="F11" s="46"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="35"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+    </row>
+    <row r="14" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A14" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="47"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+    </row>
+    <row r="15" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="37"/>
+    </row>
+    <row r="16" spans="1:6" ht="210" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>1</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>2</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>3</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="48"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+    </row>
+    <row r="20" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>1</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>2</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <v>3</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A23" s="9">
+        <v>4</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="48"/>
+      <c r="B24" s="48"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F4:F11"/>
+    <mergeCell ref="A14:F14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>